<commit_message>
-added medkit(WATERMELON) and restore health script l-imit amount of bomb and spray usage
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>To DO</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +528,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -684,6 +687,9 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -711,6 +717,9 @@
       </c>
       <c r="D15" t="s">
         <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>